<commit_message>
Limpiar encabezados y verificar datos sin NA
</commit_message>
<xml_diff>
--- a/data/infectado1_sin_suero.xlsx
+++ b/data/infectado1_sin_suero.xlsx
@@ -11,32 +11,6 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="7">
-  <si>
-    <t>Péptido</t>
-  </si>
-  <si>
-    <t>Concentración (µg/mL)</t>
-  </si>
-  <si>
-    <t>Absorbancia (450 nm)</t>
-  </si>
-  <si>
-    <t>Péptido 1</t>
-  </si>
-  <si>
-    <t>Péptido 2</t>
-  </si>
-  <si>
-    <t>Péptido 3</t>
-  </si>
-  <si>
-    <t>Péptido 4</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,27 +40,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -95,8 +54,8 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -398,20 +357,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>peptido</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>concentracion</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>absorbancia</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -420,9 +387,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B3">
         <v>0.5</v>
@@ -431,9 +400,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -442,9 +413,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -453,9 +426,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>3</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B6">
         <v>0.5</v>
@@ -464,9 +439,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -475,9 +452,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>3</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B8">
         <v>0.5</v>
@@ -486,9 +465,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>3</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B9">
         <v>0.5</v>
@@ -497,9 +478,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>3</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B10">
         <v>0.5</v>
@@ -508,9 +491,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>3</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B11">
         <v>0.5</v>
@@ -519,9 +504,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>3</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B12">
         <v>0.5</v>
@@ -530,9 +517,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>3</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B13">
         <v>0.5</v>
@@ -541,9 +530,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>3</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B14">
         <v>0.5</v>
@@ -552,9 +543,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>3</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -563,9 +556,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>3</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B16">
         <v>0.5</v>
@@ -574,9 +569,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>3</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B17">
         <v>0.5</v>
@@ -585,9 +582,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>3</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B18">
         <v>0.5</v>
@@ -596,9 +595,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>3</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B19">
         <v>0.5</v>
@@ -607,9 +608,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>3</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B20">
         <v>0.5</v>
@@ -618,9 +621,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>3</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B21">
         <v>0.5</v>
@@ -629,9 +634,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>3</v>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B22">
         <v>0.5</v>
@@ -640,9 +647,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>3</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B23">
         <v>0.5</v>
@@ -651,9 +660,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>3</v>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B24">
         <v>0.5</v>
@@ -662,9 +673,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>3</v>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B25">
         <v>0.5</v>
@@ -673,9 +686,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>3</v>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B26">
         <v>0.5</v>
@@ -684,9 +699,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>3</v>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B27">
         <v>1</v>
@@ -695,9 +712,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>3</v>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B28">
         <v>1</v>
@@ -706,9 +725,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>3</v>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B29">
         <v>1</v>
@@ -717,9 +738,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>3</v>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B30">
         <v>1</v>
@@ -728,9 +751,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>3</v>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B31">
         <v>1</v>
@@ -739,9 +764,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>3</v>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B32">
         <v>1</v>
@@ -750,9 +777,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>3</v>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B33">
         <v>1</v>
@@ -761,9 +790,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>3</v>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B34">
         <v>1</v>
@@ -772,9 +803,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>3</v>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B35">
         <v>1</v>
@@ -783,9 +816,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>3</v>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B36">
         <v>1</v>
@@ -794,9 +829,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>3</v>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B37">
         <v>1</v>
@@ -805,9 +842,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>3</v>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B38">
         <v>1</v>
@@ -816,9 +855,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>3</v>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B39">
         <v>1</v>
@@ -827,9 +868,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>3</v>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B40">
         <v>1</v>
@@ -838,9 +881,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>3</v>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B41">
         <v>1</v>
@@ -849,9 +894,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>3</v>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B42">
         <v>1</v>
@@ -860,9 +907,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>3</v>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B43">
         <v>1</v>
@@ -871,9 +920,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>3</v>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B44">
         <v>1</v>
@@ -882,9 +933,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>3</v>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B45">
         <v>1</v>
@@ -893,9 +946,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>3</v>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B46">
         <v>1</v>
@@ -904,9 +959,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>3</v>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B47">
         <v>1</v>
@@ -915,9 +972,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>3</v>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B48">
         <v>1</v>
@@ -926,9 +985,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>3</v>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B49">
         <v>1</v>
@@ -937,9 +998,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>3</v>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B50">
         <v>1</v>
@@ -948,9 +1011,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>3</v>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Péptido 1</t>
+        </is>
       </c>
       <c r="B51">
         <v>1</v>
@@ -959,9 +1024,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>4</v>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B52">
         <v>0.5</v>
@@ -970,9 +1037,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>4</v>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B53">
         <v>0.5</v>
@@ -981,9 +1050,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>4</v>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B54">
         <v>0.5</v>
@@ -992,9 +1063,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>4</v>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B55">
         <v>0.5</v>
@@ -1003,9 +1076,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>4</v>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B56">
         <v>0.5</v>
@@ -1014,9 +1089,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>4</v>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B57">
         <v>0.5</v>
@@ -1025,9 +1102,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>4</v>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B58">
         <v>0.5</v>
@@ -1036,9 +1115,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>4</v>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B59">
         <v>0.5</v>
@@ -1047,9 +1128,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>4</v>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B60">
         <v>0.5</v>
@@ -1058,9 +1141,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>4</v>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B61">
         <v>0.5</v>
@@ -1069,9 +1154,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>4</v>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B62">
         <v>0.5</v>
@@ -1080,9 +1167,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>4</v>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B63">
         <v>0.5</v>
@@ -1091,9 +1180,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>4</v>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B64">
         <v>0.5</v>
@@ -1102,9 +1193,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>4</v>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B65">
         <v>0.5</v>
@@ -1113,9 +1206,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>4</v>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B66">
         <v>0.5</v>
@@ -1124,9 +1219,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>4</v>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B67">
         <v>0.5</v>
@@ -1135,9 +1232,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>4</v>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B68">
         <v>0.5</v>
@@ -1146,9 +1245,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>4</v>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B69">
         <v>0.5</v>
@@ -1157,9 +1258,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>4</v>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B70">
         <v>0.5</v>
@@ -1168,9 +1271,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>4</v>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B71">
         <v>0.5</v>
@@ -1179,9 +1284,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>4</v>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B72">
         <v>0.5</v>
@@ -1190,9 +1297,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>4</v>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B73">
         <v>0.5</v>
@@ -1201,9 +1310,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>4</v>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B74">
         <v>0.5</v>
@@ -1212,9 +1323,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>4</v>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B75">
         <v>0.5</v>
@@ -1223,9 +1336,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>4</v>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B76">
         <v>0.5</v>
@@ -1234,9 +1349,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>4</v>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B77">
         <v>1</v>
@@ -1245,9 +1362,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>4</v>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B78">
         <v>1</v>
@@ -1256,9 +1375,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>4</v>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B79">
         <v>1</v>
@@ -1267,9 +1388,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>4</v>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B80">
         <v>1</v>
@@ -1278,9 +1401,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>4</v>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B81">
         <v>1</v>
@@ -1289,9 +1414,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>4</v>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B82">
         <v>1</v>
@@ -1300,9 +1427,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>4</v>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B83">
         <v>1</v>
@@ -1311,9 +1440,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>4</v>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B84">
         <v>1</v>
@@ -1322,9 +1453,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>4</v>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B85">
         <v>1</v>
@@ -1333,9 +1466,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>4</v>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B86">
         <v>1</v>
@@ -1344,9 +1479,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>4</v>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B87">
         <v>1</v>
@@ -1355,9 +1492,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>4</v>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B88">
         <v>1</v>
@@ -1366,9 +1505,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>4</v>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B89">
         <v>1</v>
@@ -1377,9 +1518,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
-        <v>4</v>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B90">
         <v>1</v>
@@ -1388,9 +1531,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>4</v>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B91">
         <v>1</v>
@@ -1399,9 +1544,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>4</v>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B92">
         <v>1</v>
@@ -1410,9 +1557,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>4</v>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B93">
         <v>1</v>
@@ -1421,9 +1570,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>4</v>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B94">
         <v>1</v>
@@ -1432,9 +1583,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>4</v>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B95">
         <v>1</v>
@@ -1443,9 +1596,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
-        <v>4</v>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B96">
         <v>1</v>
@@ -1454,9 +1609,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>4</v>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B97">
         <v>1</v>
@@ -1465,9 +1622,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>4</v>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B98">
         <v>1</v>
@@ -1476,9 +1635,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>4</v>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B99">
         <v>1</v>
@@ -1487,9 +1648,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>4</v>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B100">
         <v>1</v>
@@ -1498,9 +1661,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>4</v>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Péptido 2</t>
+        </is>
       </c>
       <c r="B101">
         <v>1</v>
@@ -1509,9 +1674,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>5</v>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B102">
         <v>0.5</v>
@@ -1520,9 +1687,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>5</v>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B103">
         <v>0.5</v>
@@ -1531,9 +1700,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>5</v>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B104">
         <v>0.5</v>
@@ -1542,9 +1713,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>5</v>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B105">
         <v>0.5</v>
@@ -1553,9 +1726,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>5</v>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B106">
         <v>0.5</v>
@@ -1564,9 +1739,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>5</v>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B107">
         <v>0.5</v>
@@ -1575,9 +1752,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>5</v>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B108">
         <v>0.5</v>
@@ -1586,9 +1765,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>5</v>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B109">
         <v>0.5</v>
@@ -1597,9 +1778,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>5</v>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B110">
         <v>0.5</v>
@@ -1608,9 +1791,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>5</v>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B111">
         <v>0.5</v>
@@ -1619,9 +1804,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
-      <c r="A112" t="s">
-        <v>5</v>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B112">
         <v>0.5</v>
@@ -1630,9 +1817,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>5</v>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B113">
         <v>0.5</v>
@@ -1641,9 +1830,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>5</v>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B114">
         <v>0.5</v>
@@ -1652,9 +1843,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>5</v>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B115">
         <v>0.5</v>
@@ -1663,9 +1856,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>5</v>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B116">
         <v>0.5</v>
@@ -1674,9 +1869,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>5</v>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B117">
         <v>0.5</v>
@@ -1685,9 +1882,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
-        <v>5</v>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B118">
         <v>0.5</v>
@@ -1696,9 +1895,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>5</v>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B119">
         <v>0.5</v>
@@ -1707,9 +1908,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>5</v>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B120">
         <v>0.5</v>
@@ -1718,9 +1921,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>5</v>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B121">
         <v>0.5</v>
@@ -1729,9 +1934,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>5</v>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B122">
         <v>0.5</v>
@@ -1740,9 +1947,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>5</v>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B123">
         <v>0.5</v>
@@ -1751,9 +1960,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
-      <c r="A124" t="s">
-        <v>5</v>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B124">
         <v>0.5</v>
@@ -1762,9 +1973,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
-      <c r="A125" t="s">
-        <v>5</v>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B125">
         <v>0.5</v>
@@ -1773,9 +1986,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
-      <c r="A126" t="s">
-        <v>5</v>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B126">
         <v>0.5</v>
@@ -1784,9 +1999,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
-      <c r="A127" t="s">
-        <v>5</v>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B127">
         <v>1</v>
@@ -1795,9 +2012,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
-      <c r="A128" t="s">
-        <v>5</v>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B128">
         <v>1</v>
@@ -1806,9 +2025,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
-      <c r="A129" t="s">
-        <v>5</v>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B129">
         <v>1</v>
@@ -1817,9 +2038,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
-      <c r="A130" t="s">
-        <v>5</v>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B130">
         <v>1</v>
@@ -1828,9 +2051,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
-      <c r="A131" t="s">
-        <v>5</v>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B131">
         <v>1</v>
@@ -1839,9 +2064,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
-      <c r="A132" t="s">
-        <v>5</v>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B132">
         <v>1</v>
@@ -1850,9 +2077,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
-      <c r="A133" t="s">
-        <v>5</v>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B133">
         <v>1</v>
@@ -1861,9 +2090,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
-      <c r="A134" t="s">
-        <v>5</v>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B134">
         <v>1</v>
@@ -1872,9 +2103,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
-      <c r="A135" t="s">
-        <v>5</v>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B135">
         <v>1</v>
@@ -1883,9 +2116,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
-      <c r="A136" t="s">
-        <v>5</v>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B136">
         <v>1</v>
@@ -1894,9 +2129,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
-      <c r="A137" t="s">
-        <v>5</v>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B137">
         <v>1</v>
@@ -1905,9 +2142,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
-      <c r="A138" t="s">
-        <v>5</v>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B138">
         <v>1</v>
@@ -1916,9 +2155,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
-      <c r="A139" t="s">
-        <v>5</v>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B139">
         <v>1</v>
@@ -1927,9 +2168,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
-      <c r="A140" t="s">
-        <v>5</v>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B140">
         <v>1</v>
@@ -1938,9 +2181,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
-      <c r="A141" t="s">
-        <v>5</v>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B141">
         <v>1</v>
@@ -1949,9 +2194,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
-      <c r="A142" t="s">
-        <v>5</v>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B142">
         <v>1</v>
@@ -1960,9 +2207,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
-      <c r="A143" t="s">
-        <v>5</v>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B143">
         <v>1</v>
@@ -1971,9 +2220,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
-      <c r="A144" t="s">
-        <v>5</v>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B144">
         <v>1</v>
@@ -1982,9 +2233,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
-      <c r="A145" t="s">
-        <v>5</v>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B145">
         <v>1</v>
@@ -1993,9 +2246,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
-      <c r="A146" t="s">
-        <v>5</v>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2004,9 +2259,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
-      <c r="A147" t="s">
-        <v>5</v>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2015,9 +2272,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
-      <c r="A148" t="s">
-        <v>5</v>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2026,9 +2285,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
-      <c r="A149" t="s">
-        <v>5</v>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B149">
         <v>1</v>
@@ -2037,9 +2298,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
-      <c r="A150" t="s">
-        <v>5</v>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B150">
         <v>1</v>
@@ -2048,9 +2311,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
-      <c r="A151" t="s">
-        <v>5</v>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Péptido 3</t>
+        </is>
       </c>
       <c r="B151">
         <v>1</v>
@@ -2059,9 +2324,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
-      <c r="A152" t="s">
-        <v>6</v>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B152">
         <v>0.5</v>
@@ -2070,9 +2337,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
-      <c r="A153" t="s">
-        <v>6</v>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B153">
         <v>0.5</v>
@@ -2081,9 +2350,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
-      <c r="A154" t="s">
-        <v>6</v>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B154">
         <v>0.5</v>
@@ -2092,9 +2363,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
-      <c r="A155" t="s">
-        <v>6</v>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B155">
         <v>0.5</v>
@@ -2103,9 +2376,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
-      <c r="A156" t="s">
-        <v>6</v>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B156">
         <v>0.5</v>
@@ -2114,9 +2389,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
-      <c r="A157" t="s">
-        <v>6</v>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B157">
         <v>0.5</v>
@@ -2125,9 +2402,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
-      <c r="A158" t="s">
-        <v>6</v>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B158">
         <v>0.5</v>
@@ -2136,9 +2415,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
-      <c r="A159" t="s">
-        <v>6</v>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B159">
         <v>0.5</v>
@@ -2147,9 +2428,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
-      <c r="A160" t="s">
-        <v>6</v>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B160">
         <v>0.5</v>
@@ -2158,9 +2441,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
-      <c r="A161" t="s">
-        <v>6</v>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B161">
         <v>0.5</v>
@@ -2169,9 +2454,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
-      <c r="A162" t="s">
-        <v>6</v>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B162">
         <v>0.5</v>
@@ -2180,9 +2467,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
-      <c r="A163" t="s">
-        <v>6</v>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B163">
         <v>0.5</v>
@@ -2191,9 +2480,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
-      <c r="A164" t="s">
-        <v>6</v>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B164">
         <v>0.5</v>
@@ -2202,9 +2493,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
-      <c r="A165" t="s">
-        <v>6</v>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B165">
         <v>0.5</v>
@@ -2213,9 +2506,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
-      <c r="A166" t="s">
-        <v>6</v>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B166">
         <v>0.5</v>
@@ -2224,9 +2519,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
-      <c r="A167" t="s">
-        <v>6</v>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B167">
         <v>0.5</v>
@@ -2235,9 +2532,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
-      <c r="A168" t="s">
-        <v>6</v>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B168">
         <v>0.5</v>
@@ -2246,9 +2545,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
-      <c r="A169" t="s">
-        <v>6</v>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B169">
         <v>0.5</v>
@@ -2257,9 +2558,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
-      <c r="A170" t="s">
-        <v>6</v>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B170">
         <v>0.5</v>
@@ -2268,9 +2571,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
-      <c r="A171" t="s">
-        <v>6</v>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B171">
         <v>0.5</v>
@@ -2279,9 +2584,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
-      <c r="A172" t="s">
-        <v>6</v>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B172">
         <v>0.5</v>
@@ -2290,9 +2597,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
-      <c r="A173" t="s">
-        <v>6</v>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B173">
         <v>0.5</v>
@@ -2301,9 +2610,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
-      <c r="A174" t="s">
-        <v>6</v>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B174">
         <v>0.5</v>
@@ -2312,9 +2623,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
-      <c r="A175" t="s">
-        <v>6</v>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B175">
         <v>0.5</v>
@@ -2323,9 +2636,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
-      <c r="A176" t="s">
-        <v>6</v>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B176">
         <v>0.5</v>
@@ -2334,9 +2649,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
-      <c r="A177" t="s">
-        <v>6</v>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B177">
         <v>1</v>
@@ -2345,9 +2662,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
-      <c r="A178" t="s">
-        <v>6</v>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B178">
         <v>1</v>
@@ -2356,9 +2675,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
-      <c r="A179" t="s">
-        <v>6</v>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B179">
         <v>1</v>
@@ -2367,9 +2688,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
-      <c r="A180" t="s">
-        <v>6</v>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B180">
         <v>1</v>
@@ -2378,9 +2701,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
-      <c r="A181" t="s">
-        <v>6</v>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B181">
         <v>1</v>
@@ -2389,9 +2714,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
-      <c r="A182" t="s">
-        <v>6</v>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B182">
         <v>1</v>
@@ -2400,9 +2727,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
-      <c r="A183" t="s">
-        <v>6</v>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B183">
         <v>1</v>
@@ -2411,9 +2740,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
-      <c r="A184" t="s">
-        <v>6</v>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B184">
         <v>1</v>
@@ -2422,9 +2753,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
-      <c r="A185" t="s">
-        <v>6</v>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B185">
         <v>1</v>
@@ -2433,9 +2766,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
-      <c r="A186" t="s">
-        <v>6</v>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B186">
         <v>1</v>
@@ -2444,9 +2779,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
-      <c r="A187" t="s">
-        <v>6</v>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B187">
         <v>1</v>
@@ -2455,9 +2792,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
-      <c r="A188" t="s">
-        <v>6</v>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B188">
         <v>1</v>
@@ -2466,9 +2805,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
-      <c r="A189" t="s">
-        <v>6</v>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B189">
         <v>1</v>
@@ -2477,9 +2818,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>6</v>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B190">
         <v>1</v>
@@ -2488,9 +2831,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
-      <c r="A191" t="s">
-        <v>6</v>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B191">
         <v>1</v>
@@ -2499,9 +2844,11 @@
         <v>0.038</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
-      <c r="A192" t="s">
-        <v>6</v>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B192">
         <v>1</v>
@@ -2510,9 +2857,11 @@
         <v>0.037</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
-      <c r="A193" t="s">
-        <v>6</v>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B193">
         <v>1</v>
@@ -2521,9 +2870,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
-      <c r="A194" t="s">
-        <v>6</v>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B194">
         <v>1</v>
@@ -2532,9 +2883,11 @@
         <v>0.042</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
-      <c r="A195" t="s">
-        <v>6</v>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B195">
         <v>1</v>
@@ -2543,9 +2896,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
-      <c r="A196" t="s">
-        <v>6</v>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B196">
         <v>1</v>
@@ -2554,9 +2909,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
-      <c r="A197" t="s">
-        <v>6</v>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B197">
         <v>1</v>
@@ -2565,9 +2922,11 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
-      <c r="A198" t="s">
-        <v>6</v>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B198">
         <v>1</v>
@@ -2576,9 +2935,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
-      <c r="A199" t="s">
-        <v>6</v>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B199">
         <v>1</v>
@@ -2587,9 +2948,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
-      <c r="A200" t="s">
-        <v>6</v>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B200">
         <v>1</v>
@@ -2598,9 +2961,11 @@
         <v>0.041</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
-      <c r="A201" t="s">
-        <v>6</v>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Péptido 4</t>
+        </is>
       </c>
       <c r="B201">
         <v>1</v>

</xml_diff>